<commit_message>
Added Fillo utils - Used for reading csv alternative of POI
</commit_message>
<xml_diff>
--- a/src/main/java/resources/TestData.xlsx
+++ b/src/main/java/resources/TestData.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\My Projects\APIAutomationRestAssured\src\main\java\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CF3F9F3-6B28-4F93-ABFF-8B516E4246C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D37B878-514C-4EE1-92E5-7C3D781D3C91}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{5EB32794-0C76-41EA-BA9D-01A2B0718085}"/>
   </bookViews>
@@ -412,9 +412,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A2A6D271-469E-4774-BEBC-805BD6867D36}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -443,5 +441,6 @@
     <hyperlink ref="A2" r:id="rId1" xr:uid="{6314C4D4-4232-4BB3-8D95-3E2D0156D5B3}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>